<commit_message>
cambios de Kath y Heider anadir stakeholders
</commit_message>
<xml_diff>
--- a/docRequerimientos.xlsx
+++ b/docRequerimientos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Producto" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t xml:space="preserve">Visión del producto</t>
   </si>
@@ -39,6 +39,30 @@
   </si>
   <si>
     <t xml:space="preserve">Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Paula Herrero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpaulaherrero@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Félix Urbano Uribe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">felixgabur@yahoo.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scrum Master </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ricardo Bruzual Herrera </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bruzualricardo2006@gmail.com </t>
   </si>
   <si>
     <t xml:space="preserve">Product backlog</t>
@@ -261,7 +285,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,8 +338,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -356,12 +384,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -433,18 +461,18 @@
   </sheetPr>
   <dimension ref="B1:E14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -498,23 +526,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="C10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="12"/>
@@ -535,7 +581,7 @@
       <c r="E13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="14"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -550,7 +596,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -565,18 +611,18 @@
   </sheetPr>
   <dimension ref="B1:E15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="77.7692307692308"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="15" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="15" width="8.78542510121457"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="11.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="77.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="16" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="16" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,172 +638,172 @@
       <c r="E2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="21" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="21" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="20" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-    </row>
-    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="18" t="s">
+      <c r="C10" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C11" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="21" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="C12" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="21" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="C13" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="21" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="20" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="20" t="n">
+      <c r="C14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="21" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="20" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19" t="n">
-        <v>4</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19" t="n">
-        <v>5</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="19" t="n">
-        <v>6</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="19" t="n">
-        <v>7</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="20" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="19" t="n">
-        <v>8</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="20" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="19" t="n">
-        <v>9</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="20" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="19" t="n">
-        <v>10</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="20" t="n">
-        <v>2</v>
-      </c>
-    </row>
     <row r="15" customFormat="false" ht="7.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -765,7 +811,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
agregado CRUD de admin
</commit_message>
<xml_diff>
--- a/docRequerimientos.xlsx
+++ b/docRequerimientos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Producto" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
   <si>
     <t>Visión del producto</t>
   </si>
@@ -259,6 +259,36 @@
   </si>
   <si>
     <t>reducir el tiempo de ocio de los jugadores con actividades productivas de conocimiento</t>
+  </si>
+  <si>
+    <t>yo como administrador quiero crear la ayuda para que los usuarios conozcan las reglas del juego y los retos</t>
+  </si>
+  <si>
+    <t>yo como administrador quiero modificar la ayuda para que los usuarios tengas las reglas del juego y los retos de forma actualizada</t>
+  </si>
+  <si>
+    <t>yo como administrador quiero visualizar la ayuda para verificar como se presenta al usuario las reglas del juego</t>
+  </si>
+  <si>
+    <t>yo como administrador quiero iniciar sesion en la aplicación para poder gestionar las trivias y premios</t>
+  </si>
+  <si>
+    <t>yo como usuario quiero buscar usuarios en el ranking para saber en que posicion esta un compañero</t>
+  </si>
+  <si>
+    <t>yo como administrador quiero modificar roles  para poder gestionar los privilegios</t>
+  </si>
+  <si>
+    <t>yo como administrador quiero  visualizar para conocer los usuarios de cada tipo de rol</t>
+  </si>
+  <si>
+    <t>yo como administrador quiero  eliminar  roles para poder gestionar los tipos de usuario</t>
+  </si>
+  <si>
+    <t>yo como administrador quiero crear para poder gestionar los inicios de sesion y pivilegios</t>
+  </si>
+  <si>
+    <t>yo como administrador quiero eliminar la ayuda para redefinir reglas del juego</t>
   </si>
 </sst>
 </file>
@@ -488,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -503,83 +533,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -949,49 +982,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="38.1" customHeight="1">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" ht="18.75">
-      <c r="B3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
+      <c r="B3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" ht="24" customHeight="1">
-      <c r="B4" s="13"/>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" ht="18.75">
-      <c r="B5" s="13"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:5" ht="18.75">
-      <c r="B6" s="13"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1005,113 +1038,113 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="B8" s="16"/>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="16"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1">
-      <c r="B10" s="16"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30">
       <c r="A12" s="4"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="B13" s="16"/>
-      <c r="C13" s="17" t="s">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="B14" s="16"/>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="B15" s="16"/>
-      <c r="C15" s="17" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="B16" s="22"/>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="13" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1129,19 +1162,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AMK66"/>
+  <dimension ref="A3:AMK70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="28" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="28" customWidth="1"/>
-    <col min="4" max="4" width="78.42578125" style="28" customWidth="1"/>
-    <col min="5" max="5" width="18" style="28" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="78.42578125" style="23" customWidth="1"/>
+    <col min="5" max="5" width="18" style="23" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" style="5" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="5" customWidth="1"/>
     <col min="8" max="8" width="26.28515625" style="5" customWidth="1"/>
@@ -1150,675 +1183,779 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="29.1" customHeight="1">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="2:9" ht="18" customHeight="1">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="29.85" customHeight="1">
-      <c r="B5" s="25">
+      <c r="B5" s="20">
         <v>1</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="26" t="s">
+      <c r="C5" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="26">
-        <v>2</v>
-      </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="29" t="s">
+      <c r="E5" s="21">
+        <v>2</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="24" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="27.6" customHeight="1">
-      <c r="B6" s="25">
-        <v>2</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="26" t="s">
+      <c r="B6" s="20">
+        <v>2</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="26">
-        <v>2</v>
-      </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="29" t="s">
+      <c r="E6" s="21">
+        <v>2</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="30">
-      <c r="B7" s="25">
+      <c r="B7" s="20">
         <v>3</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="C7" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="30">
-      <c r="B8" s="25">
+      <c r="B8" s="20">
         <v>4</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="26" t="s">
+      <c r="C8" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:9">
-      <c r="B9" s="25">
+      <c r="B9" s="20">
         <v>5</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="30">
-      <c r="B10" s="25">
+      <c r="B10" s="20">
         <v>6</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="30">
-      <c r="B11" s="25">
+      <c r="B11" s="20">
         <v>7</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="26" t="s">
+      <c r="C11" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="30">
-      <c r="B12" s="25">
+      <c r="B12" s="20">
         <v>8</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="26" t="s">
+      <c r="C12" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="30">
-      <c r="B13" s="25">
+      <c r="B13" s="20">
         <v>9</v>
       </c>
-      <c r="C13" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="26" t="s">
+      <c r="C13" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="30">
-      <c r="B14" s="25">
+      <c r="B14" s="20">
         <v>10</v>
       </c>
-      <c r="C14" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="26" t="s">
+      <c r="C14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="30">
-      <c r="B15" s="25">
+      <c r="B15" s="20">
         <v>11</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="30">
-      <c r="B16" s="25">
+      <c r="B16" s="20">
         <v>12</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="30">
-      <c r="B17" s="25">
+      <c r="B17" s="20">
         <v>13</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="30">
-      <c r="B18" s="25">
+      <c r="B18" s="20">
         <v>14</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="30">
-      <c r="B19" s="25">
+      <c r="B19" s="20">
         <v>15</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="30">
-      <c r="B20" s="25">
+      <c r="B20" s="20">
         <v>16</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="26" t="s">
+      <c r="C20" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="30">
-      <c r="B21" s="25">
+      <c r="B21" s="20">
         <v>17</v>
       </c>
-      <c r="C21" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="26" t="s">
+      <c r="C21" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="30">
-      <c r="B22" s="25">
+      <c r="B22" s="20">
         <v>18</v>
       </c>
-      <c r="C22" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="26" t="s">
+      <c r="C22" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="45">
-      <c r="B23" s="25">
+      <c r="B23" s="20">
         <v>19</v>
       </c>
-      <c r="C23" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="26" t="s">
+      <c r="C23" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="26">
+      <c r="E23" s="21">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="30">
-      <c r="B24" s="25">
+      <c r="B24" s="20">
         <v>20</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="30">
-      <c r="B25" s="25">
+      <c r="B25" s="20">
         <v>21</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E25" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="30">
-      <c r="B26" s="25">
+      <c r="B26" s="20">
         <v>22</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="28.35" customHeight="1">
-      <c r="B27" s="25">
+      <c r="B27" s="20">
         <v>23</v>
       </c>
-      <c r="C27" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="26" t="s">
+      <c r="C27" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="26">
+      <c r="E27" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="26.85" customHeight="1">
-      <c r="B28" s="25">
+      <c r="B28" s="20">
         <v>24</v>
       </c>
-      <c r="C28" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="26" t="s">
+      <c r="C28" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="30">
-      <c r="B29" s="25">
+      <c r="B29" s="20">
         <v>25</v>
       </c>
-      <c r="C29" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="26" t="s">
+      <c r="C29" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="26">
+      <c r="E29" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="25">
+      <c r="B30" s="20">
         <v>26</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="26">
+      <c r="E30" s="21">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="30">
-      <c r="B31" s="25">
+      <c r="B31" s="20">
         <v>27</v>
       </c>
-      <c r="C31" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="26" t="s">
+      <c r="C31" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="26"/>
+      <c r="E31" s="21"/>
     </row>
     <row r="32" spans="2:5" ht="30">
-      <c r="B32" s="25">
+      <c r="B32" s="20">
         <v>28</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E32" s="21">
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="30">
-      <c r="B33" s="25">
+      <c r="B33" s="20">
         <v>29</v>
       </c>
-      <c r="C33" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="26" t="s">
+      <c r="C33" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="26">
+      <c r="E33" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="30">
-      <c r="B34" s="25">
+      <c r="B34" s="20">
         <v>30</v>
       </c>
-      <c r="C34" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="26" t="s">
+      <c r="C34" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="26">
+      <c r="E34" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="30">
-      <c r="B35" s="25">
+      <c r="B35" s="20">
         <v>31</v>
       </c>
-      <c r="C35" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="26" t="s">
+      <c r="C35" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="26">
+      <c r="E35" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="30">
-      <c r="B36" s="25">
-        <v>32</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" s="26" t="s">
+      <c r="B36" s="20">
+        <v>32</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="26">
+      <c r="E36" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="25"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="25"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-    </row>
-    <row r="39" spans="2:5" s="5" customFormat="1">
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
+    <row r="37" spans="2:5" ht="30">
+      <c r="B37" s="32">
+        <v>33</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="30">
+      <c r="B38" s="32">
+        <v>34</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" s="5" customFormat="1" ht="30">
+      <c r="B39" s="32">
+        <v>35</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" s="21">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="2:5" s="5" customFormat="1">
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-    </row>
-    <row r="41" spans="2:5" s="5" customFormat="1">
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-    </row>
-    <row r="42" spans="2:5" s="5" customFormat="1">
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
+      <c r="B40" s="32">
+        <v>36</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" s="5" customFormat="1" ht="30">
+      <c r="B41" s="32">
+        <v>37</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" s="5" customFormat="1" ht="30">
+      <c r="B42" s="32">
+        <v>38</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" s="20">
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="2:5" s="5" customFormat="1">
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
+      <c r="B43" s="32">
+        <v>39</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="2:5" s="5" customFormat="1">
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-    </row>
-    <row r="45" spans="2:5" s="5" customFormat="1">
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-    </row>
-    <row r="46" spans="2:5" s="5" customFormat="1">
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
+      <c r="B44" s="32">
+        <v>40</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" s="5" customFormat="1" ht="30">
+      <c r="B45" s="32">
+        <v>41</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" s="5" customFormat="1" ht="30">
+      <c r="B46" s="32">
+        <v>42</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" s="20">
+        <v>2</v>
+      </c>
     </row>
     <row r="47" spans="2:5" s="5" customFormat="1">
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
     </row>
     <row r="48" spans="2:5" s="5" customFormat="1">
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
     </row>
     <row r="49" spans="2:5" s="5" customFormat="1">
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
     </row>
     <row r="50" spans="2:5" s="5" customFormat="1">
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
     </row>
     <row r="51" spans="2:5" s="5" customFormat="1">
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
     </row>
     <row r="52" spans="2:5" s="5" customFormat="1">
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
     </row>
     <row r="53" spans="2:5" s="5" customFormat="1">
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
     </row>
     <row r="54" spans="2:5" s="5" customFormat="1">
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
     </row>
     <row r="55" spans="2:5" s="5" customFormat="1">
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
     </row>
     <row r="56" spans="2:5" s="5" customFormat="1">
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
     </row>
     <row r="57" spans="2:5" s="5" customFormat="1">
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
     </row>
     <row r="58" spans="2:5" s="5" customFormat="1">
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
     </row>
     <row r="59" spans="2:5" s="5" customFormat="1">
-      <c r="B59" s="28"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="28"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
     </row>
     <row r="60" spans="2:5" s="5" customFormat="1">
-      <c r="B60" s="28"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
     </row>
     <row r="61" spans="2:5" s="5" customFormat="1">
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
     </row>
     <row r="62" spans="2:5" s="5" customFormat="1">
-      <c r="B62" s="28"/>
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
-      <c r="E62" s="28"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
     </row>
     <row r="63" spans="2:5" s="5" customFormat="1">
-      <c r="B63" s="28"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="28"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
     </row>
     <row r="64" spans="2:5" s="5" customFormat="1">
-      <c r="B64" s="28"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="28"/>
-      <c r="E64" s="28"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
     </row>
     <row r="65" spans="2:5" s="5" customFormat="1">
-      <c r="B65" s="28"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="28"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
     </row>
     <row r="66" spans="2:5" s="5" customFormat="1">
-      <c r="B66" s="28"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+    </row>
+    <row r="67" spans="2:5" s="5" customFormat="1">
+      <c r="B67" s="23"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
+    </row>
+    <row r="68" spans="2:5" s="5" customFormat="1">
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+    </row>
+    <row r="69" spans="2:5" s="5" customFormat="1">
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
+    </row>
+    <row r="70" spans="2:5" s="5" customFormat="1">
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
     </row>
   </sheetData>
   <autoFilter ref="B4:E32">

</xml_diff>

<commit_message>
agregado CRUD para admin
</commit_message>
<xml_diff>
--- a/docRequerimientos.xlsx
+++ b/docRequerimientos.xlsx
@@ -285,10 +285,10 @@
     <t>yo como administrador quiero  eliminar  roles para poder gestionar los tipos de usuario</t>
   </si>
   <si>
-    <t>yo como administrador quiero crear para poder gestionar los inicios de sesion y pivilegios</t>
-  </si>
-  <si>
     <t>yo como administrador quiero eliminar la ayuda para redefinir reglas del juego</t>
+  </si>
+  <si>
+    <t>yo como administrador quiero crear roles para poder gestionar los inicios de sesion y pivilegios</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1165,7 @@
   <dimension ref="A3:AMK70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1723,7 +1723,7 @@
         <v>32</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E40" s="21">
         <v>1</v>
@@ -1751,7 +1751,7 @@
         <v>36</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E42" s="20">
         <v>2</v>

</xml_diff>